<commit_message>
hello may not be included
</commit_message>
<xml_diff>
--- a/First.xlsx
+++ b/First.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF81E567-A315-413C-9F28-4389D38D0AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4104ED-9F24-4C22-ADCD-6945C7CA9DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -495,128 +495,171 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.109375" customWidth="1"/>
     <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="C1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="C3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="C4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="C5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="C6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="C7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="C8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="C9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="C10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="C11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="C12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="23.4" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="23.4" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>8</v>
+      </c>
+      <c r="C14">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>